<commit_message>
fire truck report, JWT on
</commit_message>
<xml_diff>
--- a/fire_station_project/report_templates/fire_truck.xlsx
+++ b/fire_station_project/report_templates/fire_truck.xlsx
@@ -1,26 +1,125 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\server\serverFireStation\fire_station_project\report_templates\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18EF3850-61C7-40E4-95E6-0FC8F81E71B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
+  <si>
+    <t>ЭКСПЛУАТАЦИОННАЯ КАРТОЧКА</t>
+  </si>
+  <si>
+    <t>Дата</t>
+  </si>
+  <si>
+    <t>Наименование и место работы автомобиля</t>
+  </si>
+  <si>
+    <t>РАБОТА ПОЖАРНОГО АВТОМОБИЛЯ</t>
+  </si>
+  <si>
+    <t>Израсходовано ГСМ, л</t>
+  </si>
+  <si>
+    <t>ИТОГО</t>
+  </si>
+  <si>
+    <t>Израсходовано ГСМ по норме, л</t>
+  </si>
+  <si>
+    <t>Израсходовано ГСМ,  л</t>
+  </si>
+  <si>
+    <t>Автомобиль:</t>
+  </si>
+  <si>
+    <t>Начало периода:</t>
+  </si>
+  <si>
+    <t>Конец периода:</t>
+  </si>
+  <si>
+    <t>Подписи</t>
+  </si>
+  <si>
+    <t>Дежурного водителя</t>
+  </si>
+  <si>
+    <t>Дежурного начальника караула</t>
+  </si>
+  <si>
+    <t>Наличие ГСМ перед выездом, л</t>
+  </si>
+  <si>
+    <t>Время выезда</t>
+  </si>
+  <si>
+    <t>Время возвращения</t>
+  </si>
+  <si>
+    <t>Показания спидометра перед выездом, км</t>
+  </si>
+  <si>
+    <t>Пройдено км к месту работы и обратно</t>
+  </si>
+  <si>
+    <t>Наличие ГСМ при при возвращении, л</t>
+  </si>
+  <si>
+    <t>Показания спидометра при возвращении, км</t>
+  </si>
+  <si>
+    <t>Экономия, л</t>
+  </si>
+  <si>
+    <t>Перерасход, л</t>
+  </si>
+  <si>
+    <t>С агрегатом</t>
+  </si>
+  <si>
+    <t>Без агрегата</t>
+  </si>
+  <si>
+    <t>Получено ГСМ, л</t>
+  </si>
+  <si>
+    <t>Наработка пожарного автомобиля, мин</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -28,16 +127,92 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color indexed="8"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -45,15 +220,136 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -330,13 +626,321 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Y6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P17" sqref="P17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="13.7109375" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" customWidth="1"/>
+    <col min="5" max="5" width="11" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" customWidth="1"/>
+    <col min="9" max="10" width="10.42578125" customWidth="1"/>
+    <col min="11" max="11" width="8.85546875" customWidth="1"/>
+    <col min="13" max="13" width="12.42578125" customWidth="1"/>
+    <col min="14" max="14" width="12.5703125" customWidth="1"/>
+    <col min="15" max="15" width="11.42578125" customWidth="1"/>
+    <col min="16" max="16" width="15.140625" customWidth="1"/>
+    <col min="17" max="17" width="14.7109375" customWidth="1"/>
+    <col min="18" max="18" width="11.42578125" customWidth="1"/>
+    <col min="19" max="19" width="13.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A1" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
+      <c r="M1" s="23"/>
+      <c r="N1" s="23"/>
+      <c r="O1" s="23"/>
+      <c r="P1" s="23"/>
+      <c r="Q1" s="23"/>
+      <c r="R1" s="23"/>
+      <c r="S1" s="23"/>
+      <c r="T1" s="23"/>
+      <c r="U1" s="23"/>
+      <c r="V1" s="9"/>
+      <c r="W1" s="9"/>
+      <c r="X1" s="9"/>
+      <c r="Y1" s="9"/>
+    </row>
+    <row r="2" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="28"/>
+      <c r="L2" s="28"/>
+      <c r="M2" s="28"/>
+      <c r="N2" s="28"/>
+      <c r="O2" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="P2" s="22"/>
+      <c r="Q2" s="22"/>
+      <c r="R2" s="22"/>
+      <c r="S2" s="22"/>
+      <c r="T2" s="22"/>
+      <c r="U2" s="22"/>
+      <c r="V2" s="1"/>
+      <c r="W2" s="1"/>
+      <c r="X2" s="1"/>
+      <c r="Y2" s="1"/>
+    </row>
+    <row r="3" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
+      <c r="J3" s="24"/>
+      <c r="K3" s="24"/>
+      <c r="L3" s="24"/>
+      <c r="M3" s="24"/>
+      <c r="N3" s="24"/>
+      <c r="O3" s="24"/>
+      <c r="P3" s="24"/>
+      <c r="Q3" s="24"/>
+      <c r="R3" s="24"/>
+      <c r="S3" s="24"/>
+      <c r="T3" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="U3" s="24"/>
+      <c r="V3" s="6"/>
+      <c r="W3" s="5"/>
+    </row>
+    <row r="4" spans="1:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="I4" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="J4" s="26"/>
+      <c r="K4" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="L4" s="29"/>
+      <c r="M4" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="N4" s="25"/>
+      <c r="O4" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="P4" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q4" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="R4" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="S4" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="T4" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="U4" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="V4" s="7"/>
+      <c r="W4" s="3"/>
+    </row>
+    <row r="5" spans="1:25" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="24"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="29"/>
+      <c r="I5" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="J5" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="K5" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="L5" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="M5" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="N5" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="O5" s="18"/>
+      <c r="P5" s="25"/>
+      <c r="Q5" s="19"/>
+      <c r="R5" s="20"/>
+      <c r="S5" s="21"/>
+      <c r="T5" s="27"/>
+      <c r="U5" s="27"/>
+      <c r="V5" s="8"/>
+      <c r="W5" s="4"/>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A6" s="12">
+        <v>1</v>
+      </c>
+      <c r="B6" s="12">
+        <v>2</v>
+      </c>
+      <c r="C6" s="13">
+        <v>3</v>
+      </c>
+      <c r="D6" s="12">
+        <v>4</v>
+      </c>
+      <c r="E6" s="12">
+        <v>5</v>
+      </c>
+      <c r="F6" s="13">
+        <v>6</v>
+      </c>
+      <c r="G6" s="12">
+        <v>7</v>
+      </c>
+      <c r="H6" s="14">
+        <v>8</v>
+      </c>
+      <c r="I6" s="12">
+        <v>9</v>
+      </c>
+      <c r="J6" s="14">
+        <v>10</v>
+      </c>
+      <c r="K6" s="14">
+        <v>11</v>
+      </c>
+      <c r="L6" s="14">
+        <v>12</v>
+      </c>
+      <c r="M6" s="13">
+        <v>13</v>
+      </c>
+      <c r="N6" s="13">
+        <v>14</v>
+      </c>
+      <c r="O6" s="15">
+        <v>15</v>
+      </c>
+      <c r="P6" s="13">
+        <v>16</v>
+      </c>
+      <c r="Q6" s="13">
+        <v>17</v>
+      </c>
+      <c r="R6" s="15">
+        <v>18</v>
+      </c>
+      <c r="S6" s="16">
+        <v>19</v>
+      </c>
+      <c r="T6" s="12">
+        <v>20</v>
+      </c>
+      <c r="U6" s="12">
+        <v>21</v>
+      </c>
+      <c r="V6" s="2"/>
+      <c r="W6" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="27">
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="A1:U1"/>
+    <mergeCell ref="A3:S3"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="T4:T5"/>
+    <mergeCell ref="U4:U5"/>
+    <mergeCell ref="P4:P5"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="K2:N2"/>
+    <mergeCell ref="T3:U3"/>
+    <mergeCell ref="O4:O5"/>
+    <mergeCell ref="Q4:Q5"/>
+    <mergeCell ref="R4:R5"/>
+    <mergeCell ref="S4:S5"/>
+    <mergeCell ref="O2:Q2"/>
+    <mergeCell ref="R2:U2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="51" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>